<commit_message>
[ISP-2]Nuovi attributi Profondità e Fourilista
</commit_message>
<xml_diff>
--- a/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/01_UoM.xlsx
+++ b/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/01_UoM.xlsx
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="81">
   <si>
     <t>Action</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Lower Threshold</t>
+  </si>
+  <si>
+    <t>EUR2</t>
   </si>
 </sst>
 </file>
@@ -564,6 +567,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -612,6 +663,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -653,6 +752,54 @@
             <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
@@ -926,9 +1073,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1423,6 +1572,20 @@
       </c>
       <c r="D35" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>